<commit_message>
Major update with model averaging.  Second set of files.
</commit_message>
<xml_diff>
--- a/SSDexample.xlsx
+++ b/SSDexample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carrGJ/Documents/ShinyByGIT/SSDV2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pgone-my.sharepoint.com/personal/connors_ka_pg_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4E6D0C8-2F10-974B-A58E-DDB4C19F4925}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C6CBC90-521E-402C-B132-98394093F017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="2500" windowWidth="27240" windowHeight="16440" xr2:uid="{5400004A-FFC7-F440-B65F-08C2AEB3E83A}"/>
+    <workbookView xWindow="-27885" yWindow="2790" windowWidth="24915" windowHeight="13620" xr2:uid="{5400004A-FFC7-F440-B65F-08C2AEB3E83A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -201,9 +200,6 @@
     <t>Chlorella kessleri</t>
   </si>
   <si>
-    <t>amphib</t>
-  </si>
-  <si>
     <t>C. kessleri</t>
   </si>
   <si>
@@ -235,6 +231,9 @@
   </si>
   <si>
     <t>S19</t>
+  </si>
+  <si>
+    <t>macrophyte</t>
   </si>
 </sst>
 </file>
@@ -589,12 +588,12 @@
   <dimension ref="B2:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -614,7 +613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -625,7 +624,7 @@
         <v>0.23</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -634,7 +633,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -645,7 +644,7 @@
         <v>0.24</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -654,7 +653,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -665,7 +664,7 @@
         <v>0.25</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
@@ -674,7 +673,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -685,7 +684,7 @@
         <v>0.35</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -694,7 +693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -714,7 +713,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>23</v>
       </c>
@@ -725,7 +724,7 @@
         <v>0.88</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
@@ -734,7 +733,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -745,7 +744,7 @@
         <v>0.96</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
         <v>27</v>
@@ -754,7 +753,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>29</v>
       </c>
@@ -765,7 +764,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
         <v>30</v>
@@ -774,7 +773,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>32</v>
       </c>
@@ -794,7 +793,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>35</v>
       </c>
@@ -805,7 +804,7 @@
         <v>1.35</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
         <v>37</v>
@@ -814,7 +813,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>39</v>
       </c>
@@ -825,7 +824,7 @@
         <v>1.66</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
         <v>40</v>
@@ -834,7 +833,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>42</v>
       </c>
@@ -854,7 +853,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>45</v>
       </c>
@@ -865,7 +864,7 @@
         <v>2.4</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
         <v>46</v>
@@ -874,7 +873,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>48</v>
       </c>
@@ -885,7 +884,7 @@
         <v>2.62</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
         <v>49</v>
@@ -894,7 +893,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>51</v>
       </c>
@@ -905,7 +904,7 @@
         <v>2.75</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F17" t="s">
         <v>52</v>
@@ -914,7 +913,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>54</v>
       </c>
@@ -925,18 +924,18 @@
         <v>3.5</v>
       </c>
       <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
         <v>55</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>56</v>
       </c>
-      <c r="G18" t="s">
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>58</v>
       </c>
       <c r="C19">
         <v>17</v>
@@ -945,18 +944,18 @@
         <v>3.81</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="F19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" t="s">
         <v>59</v>
       </c>
-      <c r="G19" t="s">
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>61</v>
       </c>
       <c r="C20">
         <v>18</v>
@@ -965,18 +964,18 @@
         <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="F20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" t="s">
         <v>62</v>
       </c>
-      <c r="G20" t="s">
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>64</v>
       </c>
       <c r="C21">
         <v>19</v>
@@ -985,16 +984,17 @@
         <v>15.06</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="F21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" t="s">
         <v>65</v>
-      </c>
-      <c r="G21" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>